<commit_message>
added reference row to sheet spatial
</commit_message>
<xml_diff>
--- a/dieterpy/templates/data_input/static_input.xlsx
+++ b/dieterpy/templates/data_input/static_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TUB\02_Git\dieterpy\dieterpy\templates\data_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C5DFE9-5636-4FDD-8A11-D04D97E8EE75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F5E195-7129-4091-8859-B64C76FE047F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="741" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="741" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LICENSE" sheetId="1" r:id="rId1"/>
@@ -48,91 +48,92 @@
     <author xml:space="preserve"> </author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="Times New Roman"/>
+            <family val="1"/>
           </rPr>
           <t xml:space="preserve">For GUSS tool in GAMS. When min and max are equal, we have to add a little gap
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="E16" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="E17" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Just a placeholder value; not relevant if NTCs are fixed</t>
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="E18" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Just a placeholder value; not relevant if NTCs are fixed</t>
         </r>
       </text>
     </comment>
-    <comment ref="E18" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="E19" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Just a placeholder value; not relevant if NTCs are fixed</t>
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="E20" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Just a placeholder value; not relevant if NTCs are fixed</t>
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="E21" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Just a placeholder value; not relevant if NTCs are fixed</t>
         </r>
       </text>
     </comment>
-    <comment ref="E21" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="E22" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Just a placeholder value; not relevant if NTCs are fixed</t>
         </r>
@@ -157,7 +158,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -166,7 +167,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>2030 assumptions</t>
         </r>
@@ -179,7 +180,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -187,7 +188,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Bogdanov et al. for wind and solar (2030 assumptions)</t>
@@ -201,7 +202,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -210,7 +211,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>2030 assumptions</t>
         </r>
@@ -222,6 +223,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Times New Roman"/>
+            <family val="1"/>
           </rPr>
           <t>For GUSS tool in GAMS. When min and max are equal, we have to add a little gap</t>
         </r>
@@ -234,7 +236,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -242,7 +244,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Including cpacity reserve</t>
@@ -256,7 +258,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -264,7 +266,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Including cpacity reserve</t>
@@ -278,7 +280,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -286,7 +288,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 average of hc and CCGT</t>
@@ -300,7 +302,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -308,7 +310,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 biomass + other renewables</t>
@@ -322,7 +324,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -330,7 +332,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 biomass + other renewables</t>
@@ -344,7 +346,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -352,7 +354,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 biomass + other renewables</t>
@@ -366,7 +368,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -374,7 +376,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 2030, rooftop - industrial</t>
@@ -388,7 +390,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -396,7 +398,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 average of hc and CCGT</t>
@@ -410,7 +412,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -418,7 +420,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 average of hc and CCGT</t>
@@ -432,7 +434,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -440,7 +442,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 average of hc and CCGT</t>
@@ -454,7 +456,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -462,7 +464,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 average of hc and CCGT</t>
@@ -476,7 +478,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -484,7 +486,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 average of hc and CCGT</t>
@@ -498,7 +500,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -506,7 +508,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 average of hc and CCGT</t>
@@ -520,7 +522,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -528,7 +530,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 average of hc and CCGT</t>
@@ -542,7 +544,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -550,7 +552,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 average of hc and CCGT</t>
@@ -564,7 +566,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -572,7 +574,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 average of hc and CCGT</t>
@@ -586,7 +588,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -595,7 +597,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>including solar thermal</t>
         </r>
@@ -608,7 +610,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -617,7 +619,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>including solar thermal</t>
         </r>
@@ -630,7 +632,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -638,7 +640,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 average of hc and CCGT</t>
@@ -652,7 +654,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -661,7 +663,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>including solar thermal</t>
         </r>
@@ -674,7 +676,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -683,7 +685,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>including solar thermal</t>
         </r>
@@ -696,7 +698,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -704,7 +706,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 average of hc and CCGT</t>
@@ -728,6 +730,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Times New Roman"/>
+            <family val="1"/>
           </rPr>
           <t xml:space="preserve">For GUSS tool in GAMS. When min and max are equal, we have to add a little gap
 </t>
@@ -740,6 +743,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Times New Roman"/>
+            <family val="1"/>
           </rPr>
           <t>For GUSS tool in GAMS. When min and max are equal, we have to add a little gap</t>
         </r>
@@ -752,7 +756,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -761,7 +765,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>31.9 in table 6-10, but most likely a typo</t>
         </r>
@@ -774,7 +778,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -783,7 +787,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>31.9 in table 6-10, but most likely a typo</t>
         </r>
@@ -796,7 +800,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -805,7 +809,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>31.9 in table 6-10, but most likely a typo</t>
         </r>
@@ -818,7 +822,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -827,7 +831,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>31.9 in table 6-10, but most likely a typo</t>
         </r>
@@ -840,7 +844,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -849,7 +853,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>31.9 in table 6-10, but most likely a typo</t>
         </r>
@@ -862,7 +866,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -871,7 +875,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>31.9 in table 6-10, but most likely a typo</t>
         </r>
@@ -884,7 +888,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -893,7 +897,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>31.9 in table 6-10, but most likely a typo</t>
         </r>
@@ -906,7 +910,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -915,7 +919,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>31.9 in table 6-10, but most likely a typo</t>
         </r>
@@ -928,7 +932,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -937,7 +941,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>31.9 in table 6-10, but most likely a typo</t>
         </r>
@@ -950,7 +954,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -959,7 +963,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>31.9 in table 6-10, but most likely a typo</t>
         </r>
@@ -972,7 +976,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -981,7 +985,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>31.9 in table 6-10, but most likely a typo</t>
         </r>
@@ -994,7 +998,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Author:
 </t>
@@ -1003,7 +1007,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>31.9 in table 6-10, but most likely a typo</t>
         </r>
@@ -1026,6 +1030,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Times New Roman"/>
+            <family val="1"/>
           </rPr>
           <t>For GUSS tool in GAMS. When min and max are equal, we have to add a little gap</t>
         </r>
@@ -1037,6 +1042,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="Times New Roman"/>
+            <family val="1"/>
           </rPr>
           <t>For GUSS tool in GAMS. When min and max are equal, we have to add a little gap</t>
         </r>
@@ -1049,7 +1055,7 @@
             <b/>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Schill, Wolf-Peter:</t>
         </r>
@@ -1057,7 +1063,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Assuming E/P 500</t>
@@ -1069,7 +1075,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3206" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3216" uniqueCount="603">
   <si>
     <t>This work is licensed under the Creative Commons Attribution-ShareAlike 4.0 International Public License.</t>
   </si>
@@ -2391,9 +2397,6 @@
     <t>spatial</t>
   </si>
   <si>
-    <t>N2</t>
-  </si>
-  <si>
     <t>set</t>
   </si>
   <si>
@@ -2559,9 +2562,6 @@
     <t>inc</t>
   </si>
   <si>
-    <t>M2</t>
-  </si>
-  <si>
     <t>ev_data</t>
   </si>
   <si>
@@ -2869,6 +2869,21 @@
   </si>
   <si>
     <t>Oliver Schmidt, Sylvain Melchior, Adam Hawkes, Iain Staffell</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>own assumptions</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>N3</t>
+  </si>
+  <si>
+    <t>B4</t>
   </si>
 </sst>
 </file>
@@ -2876,10 +2891,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="mmm\-yy"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="mmm\-yy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2890,37 +2905,37 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="8"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2928,36 +2943,32 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Segoe UI"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <name val="Segoe UI"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3054,7 +3065,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3074,7 +3085,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3096,10 +3107,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3125,7 +3136,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3139,17 +3150,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3182,7 +3193,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3212,7 +3223,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3221,9 +3232,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -10623,8 +10635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -10664,8 +10676,8 @@
       <c r="B2" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>440</v>
+      <c r="C2" s="61" t="s">
+        <v>601</v>
       </c>
       <c r="D2" s="9">
         <v>0</v>
@@ -10674,18 +10686,18 @@
         <v>1</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>442</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>443</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>444</v>
       </c>
       <c r="D3" s="9">
         <v>1</v>
@@ -10694,18 +10706,18 @@
         <v>0</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>445</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>443</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>446</v>
       </c>
       <c r="D4" s="9">
         <v>0</v>
@@ -10714,18 +10726,18 @@
         <v>1</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>447</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>443</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>448</v>
       </c>
       <c r="D5" s="9">
         <v>1</v>
@@ -10734,18 +10746,18 @@
         <v>0</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>449</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>443</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>450</v>
       </c>
       <c r="D6" s="9">
         <v>1</v>
@@ -10754,18 +10766,18 @@
         <v>0</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>305</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D7" s="9">
         <v>1</v>
@@ -10774,18 +10786,18 @@
         <v>0</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>305</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D8" s="9">
         <v>0</v>
@@ -10794,7 +10806,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -10802,10 +10814,10 @@
         <v>157</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D9" s="9">
         <v>1</v>
@@ -10814,18 +10826,18 @@
         <v>0</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D10" s="9">
         <v>0</v>
@@ -10834,18 +10846,18 @@
         <v>1</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>171</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D11" s="9">
         <v>1</v>
@@ -10854,18 +10866,18 @@
         <v>0</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>171</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D12" s="9">
         <v>0</v>
@@ -10874,18 +10886,18 @@
         <v>1</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>171</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D13" s="9">
         <v>1</v>
@@ -10894,18 +10906,18 @@
         <v>0</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>461</v>
+      <c r="C14" s="61" t="s">
+        <v>602</v>
       </c>
       <c r="D14" s="9">
         <v>1</v>
@@ -10914,18 +10926,18 @@
         <v>0</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>463</v>
+      <c r="C15" s="61" t="s">
+        <v>460</v>
       </c>
       <c r="D15" s="9">
         <v>0</v>
@@ -10934,18 +10946,18 @@
         <v>1</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>199</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D16" s="9">
         <v>1</v>
@@ -10954,18 +10966,18 @@
         <v>0</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>199</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D17" s="9">
         <v>0</v>
@@ -10974,18 +10986,18 @@
         <v>1</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>466</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>467</v>
-      </c>
       <c r="C18" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D18" s="9">
         <v>0</v>
@@ -10994,18 +11006,18 @@
         <v>1</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>468</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>467</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>469</v>
       </c>
       <c r="D19" s="9">
         <v>0</v>
@@ -11014,18 +11026,18 @@
         <v>1</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D20" s="9">
         <v>1</v>
@@ -11034,18 +11046,18 @@
         <v>0</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>471</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>470</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>472</v>
       </c>
       <c r="D21" s="9">
         <v>0</v>
@@ -11054,18 +11066,18 @@
         <v>1</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D22" s="9">
         <v>1</v>
@@ -11074,18 +11086,18 @@
         <v>0</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D23" s="9">
         <v>1</v>
@@ -11094,18 +11106,18 @@
         <v>0</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>475</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>470</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>476</v>
       </c>
       <c r="D24" s="9">
         <v>1</v>
@@ -11114,18 +11126,18 @@
         <v>0</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>477</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>478</v>
-      </c>
       <c r="C25" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D25" s="9">
         <v>1</v>
@@ -11134,18 +11146,18 @@
         <v>0</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D26" s="9">
         <v>1</v>
@@ -11154,18 +11166,18 @@
         <v>0</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D27" s="9">
         <v>1</v>
@@ -11174,18 +11186,18 @@
         <v>0</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D28" s="9">
         <v>1</v>
@@ -11194,18 +11206,18 @@
         <v>0</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>482</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>483</v>
       </c>
       <c r="D29" s="9">
         <v>1</v>
@@ -11214,18 +11226,18 @@
         <v>0</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>484</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>485</v>
       </c>
       <c r="D30" s="9">
         <v>1</v>
@@ -11234,18 +11246,18 @@
         <v>0</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>486</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>487</v>
       </c>
       <c r="D31" s="9">
         <v>0</v>
@@ -11254,18 +11266,18 @@
         <v>1</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>488</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>443</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>489</v>
       </c>
       <c r="D32" s="9">
         <v>4</v>
@@ -11274,18 +11286,18 @@
         <v>1</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>305</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D33" s="9">
         <v>2</v>
@@ -11294,18 +11306,18 @@
         <v>1</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D34" s="9">
         <v>2</v>
@@ -11314,18 +11326,18 @@
         <v>1</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>171</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D35" s="9">
         <v>3</v>
@@ -11334,18 +11346,18 @@
         <v>1</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>463</v>
+      <c r="C36" s="61" t="s">
+        <v>460</v>
       </c>
       <c r="D36" s="9">
         <v>1</v>
@@ -11354,18 +11366,18 @@
         <v>1</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>496</v>
+      <c r="C37" s="61" t="s">
+        <v>600</v>
       </c>
       <c r="D37" s="9">
         <v>1</v>
@@ -11374,18 +11386,18 @@
         <v>1</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="9" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>199</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D38" s="9">
         <v>1</v>
@@ -11394,18 +11406,18 @@
         <v>1</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="9" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D39" s="9">
         <v>2</v>
@@ -11414,18 +11426,18 @@
         <v>1</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="9" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D40" s="9">
         <v>2</v>
@@ -11434,18 +11446,18 @@
         <v>1</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="9" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D41" s="9">
         <v>5</v>
@@ -11454,18 +11466,18 @@
         <v>1</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="9" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D42" s="9">
         <v>7</v>
@@ -11474,18 +11486,18 @@
         <v>1</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="9" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D43" s="9">
         <v>0</v>
@@ -11494,18 +11506,18 @@
         <v>1</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="9" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B44" s="9" t="s">
+        <v>503</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>505</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>507</v>
       </c>
       <c r="D44" s="9">
         <v>1</v>
@@ -11514,18 +11526,18 @@
         <v>1</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>507</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>508</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>509</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>510</v>
       </c>
       <c r="D45" s="9">
         <v>1</v>
@@ -11534,18 +11546,18 @@
         <v>0</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="9" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D46" s="9">
         <v>1</v>
@@ -11554,7 +11566,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -11567,8 +11579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A2:AMJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="A4:XFD4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -11587,105 +11599,105 @@
   <sheetData>
     <row r="2" spans="2:10">
       <c r="B2" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>513</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>517</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>518</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>519</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="36.75" customHeight="1">
       <c r="B3" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>522</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>524</v>
       </c>
       <c r="H3" s="1">
         <v>2013</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="36.75" customHeight="1">
       <c r="B4" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>595</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>525</v>
-      </c>
-      <c r="C4" s="60" t="s">
-        <v>597</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>527</v>
       </c>
       <c r="H4" s="1">
         <v>2019</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="36.75" customHeight="1">
       <c r="B5" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>529</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>531</v>
       </c>
       <c r="H5" s="1">
         <v>2012</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="36.75" customHeight="1">
       <c r="B6" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>533</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>535</v>
       </c>
       <c r="H6" s="1">
         <v>2012</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="36.75" customHeight="1">
@@ -11693,45 +11705,45 @@
         <v>158</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>537</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>539</v>
       </c>
       <c r="H7" s="1">
         <v>2014</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="36.75" customHeight="1">
       <c r="B8" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>541</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>542</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>544</v>
       </c>
       <c r="F8" s="1">
         <v>67</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="H8" s="1">
         <v>2014</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="36.75" customHeight="1">
@@ -11739,53 +11751,53 @@
         <v>187</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>547</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>549</v>
       </c>
       <c r="H9" s="1">
         <v>2014</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="36.75" customHeight="1">
       <c r="B10" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>554</v>
       </c>
       <c r="H10" s="1">
         <v>2007</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="36.75" customHeight="1">
       <c r="B11" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>557</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>558</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>559</v>
       </c>
       <c r="F11" s="1">
         <v>92</v>
@@ -11794,109 +11806,109 @@
         <v>2017</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="36.75" customHeight="1">
       <c r="B12" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>562</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>563</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>564</v>
       </c>
       <c r="H12" s="1">
         <v>2018</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="36.75" customHeight="1">
       <c r="B13" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="I13" s="8" t="s">
         <v>567</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="36.75" customHeight="1">
       <c r="B14" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>571</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>572</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>573</v>
       </c>
       <c r="H14" s="1">
         <v>2014</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="36.75" customHeight="1">
       <c r="B15" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="I15" s="8" t="s">
         <v>576</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="J15" s="2" t="s">
         <v>577</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>578</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="36.75" customHeight="1">
       <c r="B16" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="H16" s="1">
         <v>2018</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="36.75" customHeight="1">
       <c r="B17" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>583</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>585</v>
       </c>
       <c r="F17" s="1">
         <v>68</v>
@@ -11905,7 +11917,7 @@
         <v>2013</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="36.75" customHeight="1">
@@ -11913,39 +11925,39 @@
         <v>48</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="H18" s="1">
         <v>2012</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="36.75" customHeight="1">
       <c r="B19" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>591</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>592</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>593</v>
       </c>
       <c r="H19" s="1">
         <v>2013</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="42.75" customHeight="1"/>
@@ -11987,10 +11999,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:AMJ21"/>
+  <dimension ref="A2:AMJ22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.6640625" defaultRowHeight="14.4"/>
@@ -11998,137 +12010,128 @@
     <col min="1" max="1" width="2.6640625" style="24" customWidth="1"/>
     <col min="2" max="2" width="9.88671875" style="24" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="24" customWidth="1"/>
-    <col min="5" max="7" width="9.88671875" style="24" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" style="24" customWidth="1"/>
-    <col min="9" max="10" width="9.88671875" style="24" customWidth="1"/>
-    <col min="11" max="11" width="12.88671875" style="24" customWidth="1"/>
+    <col min="4" max="10" width="11.5546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="24" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="0.88671875" style="59" customWidth="1"/>
     <col min="13" max="13" width="4.109375" style="24" customWidth="1"/>
     <col min="14" max="1023" width="6.6640625" style="24"/>
     <col min="1024" max="1024" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:1024" s="1" customFormat="1" ht="62.25" customHeight="1">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:1024">
+      <c r="B2" s="24" t="s">
+        <v>598</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="3" spans="2:1024" s="1" customFormat="1" ht="62.25" customHeight="1">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="N2" s="1" t="s">
+      <c r="L3" s="30"/>
+      <c r="N3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AMJ2"/>
-    </row>
-    <row r="3" spans="2:1024">
-      <c r="B3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="24">
-        <v>4500</v>
-      </c>
-      <c r="D3" s="24">
-        <v>4500.1000000000004</v>
-      </c>
-      <c r="E3" s="24">
-        <v>462</v>
-      </c>
-      <c r="F3" s="24">
-        <v>6000</v>
-      </c>
-      <c r="G3" s="24">
-        <v>0</v>
-      </c>
-      <c r="I3" s="24">
-        <v>35</v>
-      </c>
-      <c r="J3" s="24">
-        <v>0.04</v>
-      </c>
-      <c r="K3" s="48">
-        <v>4500</v>
-      </c>
-      <c r="M3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="24">
-        <v>1</v>
-      </c>
-      <c r="O3" s="24">
-        <v>-1</v>
-      </c>
+      <c r="AMJ3"/>
     </row>
     <row r="4" spans="2:1024">
       <c r="B4" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="24">
-        <v>3592.5</v>
+        <v>4500</v>
       </c>
       <c r="D4" s="24">
-        <v>3592.6</v>
+        <v>4500.1000000000004</v>
       </c>
       <c r="E4" s="24">
-        <v>573</v>
+        <v>462</v>
       </c>
       <c r="F4" s="24">
         <v>6000</v>
@@ -12143,30 +12146,30 @@
         <v>0.04</v>
       </c>
       <c r="K4" s="48">
-        <v>3592.5</v>
+        <v>4500</v>
       </c>
       <c r="M4" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N4" s="24">
         <v>1</v>
       </c>
-      <c r="P4" s="24">
+      <c r="O4" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="5" spans="2:1024">
       <c r="B5" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="24">
-        <v>1000</v>
+        <v>3592.5</v>
       </c>
       <c r="D5" s="24">
-        <v>1000.1</v>
+        <v>3592.6</v>
       </c>
       <c r="E5" s="24">
-        <v>343</v>
+        <v>573</v>
       </c>
       <c r="F5" s="24">
         <v>6000</v>
@@ -12181,30 +12184,30 @@
         <v>0.04</v>
       </c>
       <c r="K5" s="48">
-        <v>1000</v>
+        <v>3592.5</v>
       </c>
       <c r="M5" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N5" s="24">
         <v>1</v>
       </c>
-      <c r="Q5" s="24">
+      <c r="P5" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="6" spans="2:1024">
       <c r="B6" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="24">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="D6" s="24">
-        <v>5000.1000000000004</v>
+        <v>1000.1</v>
       </c>
       <c r="E6" s="24">
-        <v>326</v>
+        <v>343</v>
       </c>
       <c r="F6" s="24">
         <v>6000</v>
@@ -12219,30 +12222,30 @@
         <v>0.04</v>
       </c>
       <c r="K6" s="48">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N6" s="24">
         <v>1</v>
       </c>
-      <c r="R6" s="24">
+      <c r="Q6" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="7" spans="2:1024">
       <c r="B7" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="24">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="D7" s="24">
-        <v>2500.1</v>
+        <v>5000.1000000000004</v>
       </c>
       <c r="E7" s="24">
-        <v>659</v>
+        <v>326</v>
       </c>
       <c r="F7" s="24">
         <v>6000</v>
@@ -12257,30 +12260,30 @@
         <v>0.04</v>
       </c>
       <c r="K7" s="48">
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N7" s="24">
         <v>1</v>
       </c>
-      <c r="S7" s="24">
+      <c r="R7" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="8" spans="2:1024">
       <c r="B8" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="24">
-        <v>2300</v>
+        <v>2500</v>
       </c>
       <c r="D8" s="24">
-        <v>2300.1</v>
+        <v>2500.1</v>
       </c>
       <c r="E8" s="24">
-        <v>399</v>
+        <v>659</v>
       </c>
       <c r="F8" s="24">
         <v>6000</v>
@@ -12295,30 +12298,30 @@
         <v>0.04</v>
       </c>
       <c r="K8" s="48">
-        <v>2300</v>
+        <v>2500</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N8" s="24">
         <v>1</v>
       </c>
-      <c r="T8" s="24">
+      <c r="S8" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="2:1024">
       <c r="B9" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="24">
-        <v>7500</v>
+        <v>2300</v>
       </c>
       <c r="D9" s="24">
-        <v>7500.1</v>
+        <v>2300.1</v>
       </c>
       <c r="E9" s="24">
-        <v>464</v>
+        <v>399</v>
       </c>
       <c r="F9" s="24">
         <v>6000</v>
@@ -12333,30 +12336,30 @@
         <v>0.04</v>
       </c>
       <c r="K9" s="48">
-        <v>7500</v>
+        <v>2300</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N9" s="24">
         <v>1</v>
       </c>
-      <c r="U9" s="24">
+      <c r="T9" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="10" spans="2:1024">
       <c r="B10" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="24">
-        <v>4450</v>
+        <v>7500</v>
       </c>
       <c r="D10" s="24">
-        <v>4450.1000000000004</v>
+        <v>7500.1</v>
       </c>
       <c r="E10" s="24">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F10" s="24">
         <v>6000</v>
@@ -12371,30 +12374,30 @@
         <v>0.04</v>
       </c>
       <c r="K10" s="48">
-        <v>4450</v>
+        <v>7500</v>
       </c>
       <c r="M10" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N10" s="24">
         <v>1</v>
       </c>
-      <c r="V10" s="24">
+      <c r="U10" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="11" spans="2:1024">
       <c r="B11" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="24">
-        <v>3550</v>
+        <v>4450</v>
       </c>
       <c r="D11" s="24">
-        <v>3550.1</v>
+        <v>4450.1000000000004</v>
       </c>
       <c r="E11" s="24">
-        <v>443</v>
+        <v>466</v>
       </c>
       <c r="F11" s="24">
         <v>6000</v>
@@ -12409,30 +12412,30 @@
         <v>0.04</v>
       </c>
       <c r="K11" s="48">
-        <v>3550</v>
+        <v>4450</v>
       </c>
       <c r="M11" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="O11" s="24">
+        <v>30</v>
+      </c>
+      <c r="N11" s="24">
         <v>1</v>
       </c>
-      <c r="Q11" s="24">
+      <c r="V11" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="12" spans="2:1024">
       <c r="B12" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="24">
-        <v>3400</v>
+        <v>3550</v>
       </c>
       <c r="D12" s="24">
-        <v>3400.1</v>
+        <v>3550.1</v>
       </c>
       <c r="E12" s="24">
-        <v>168</v>
+        <v>443</v>
       </c>
       <c r="F12" s="24">
         <v>6000</v>
@@ -12447,30 +12450,30 @@
         <v>0.04</v>
       </c>
       <c r="K12" s="48">
-        <v>3400</v>
+        <v>3550</v>
       </c>
       <c r="M12" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="O12" s="24">
+        <v>1</v>
       </c>
       <c r="Q12" s="24">
-        <v>1</v>
-      </c>
-      <c r="R12" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="13" spans="2:1024">
       <c r="B13" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="24">
-        <v>600</v>
+        <v>3400</v>
       </c>
       <c r="D13" s="24">
-        <v>600.1</v>
+        <v>3400.1</v>
       </c>
       <c r="E13" s="24">
-        <v>332</v>
+        <v>168</v>
       </c>
       <c r="F13" s="24">
         <v>6000</v>
@@ -12485,30 +12488,30 @@
         <v>0.04</v>
       </c>
       <c r="K13" s="48">
-        <v>600</v>
+        <v>3400</v>
       </c>
       <c r="M13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="S13" s="24">
+        <v>32</v>
+      </c>
+      <c r="Q13" s="24">
         <v>1</v>
       </c>
-      <c r="T13" s="24">
+      <c r="R13" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="14" spans="2:1024">
       <c r="B14" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="24">
-        <v>1100</v>
+        <v>600</v>
       </c>
       <c r="D14" s="24">
-        <v>1100.0999999999999</v>
+        <v>600.1</v>
       </c>
       <c r="E14" s="24">
-        <v>599</v>
+        <v>332</v>
       </c>
       <c r="F14" s="24">
         <v>6000</v>
@@ -12523,30 +12526,30 @@
         <v>0.04</v>
       </c>
       <c r="K14" s="48">
-        <v>1100</v>
+        <v>600</v>
       </c>
       <c r="M14" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="S14" s="24">
+        <v>1</v>
       </c>
       <c r="T14" s="24">
-        <v>1</v>
-      </c>
-      <c r="U14" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="15" spans="2:1024">
       <c r="B15" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="24">
-        <v>1700</v>
+        <v>1100</v>
       </c>
       <c r="D15" s="24">
-        <v>1700.1</v>
+        <v>1100.0999999999999</v>
       </c>
       <c r="E15" s="24">
-        <v>395</v>
+        <v>599</v>
       </c>
       <c r="F15" s="24">
         <v>6000</v>
@@ -12561,30 +12564,30 @@
         <v>0.04</v>
       </c>
       <c r="K15" s="48">
-        <v>1700</v>
+        <v>1100</v>
       </c>
       <c r="M15" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="T15" s="24">
+        <v>1</v>
       </c>
       <c r="U15" s="24">
-        <v>1</v>
-      </c>
-      <c r="V15" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="16" spans="2:1024">
       <c r="B16" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="24">
-        <v>2500</v>
+        <v>1700</v>
       </c>
       <c r="D16" s="24">
-        <v>2500.1</v>
-      </c>
-      <c r="E16" s="49">
-        <v>1000</v>
+        <v>1700.1</v>
+      </c>
+      <c r="E16" s="24">
+        <v>395</v>
       </c>
       <c r="F16" s="24">
         <v>6000</v>
@@ -12599,12 +12602,12 @@
         <v>0.04</v>
       </c>
       <c r="K16" s="48">
-        <v>2500</v>
+        <v>1700</v>
       </c>
       <c r="M16" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="O16" s="24">
+        <v>35</v>
+      </c>
+      <c r="U16" s="24">
         <v>1</v>
       </c>
       <c r="V16" s="24">
@@ -12613,13 +12616,13 @@
     </row>
     <row r="17" spans="2:25">
       <c r="B17" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="24">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="D17" s="24">
-        <v>5000.1000000000004</v>
+        <v>2500.1</v>
       </c>
       <c r="E17" s="49">
         <v>1000</v>
@@ -12637,27 +12640,27 @@
         <v>0.04</v>
       </c>
       <c r="K17" s="48">
-        <v>5000</v>
+        <v>2500</v>
       </c>
       <c r="M17" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O17" s="24">
         <v>1</v>
       </c>
-      <c r="W17" s="24">
+      <c r="V17" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="18" spans="2:25">
       <c r="B18" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="24">
-        <v>3255</v>
+        <v>5000</v>
       </c>
       <c r="D18" s="24">
-        <v>3255.1</v>
+        <v>5000.1000000000004</v>
       </c>
       <c r="E18" s="49">
         <v>1000</v>
@@ -12675,27 +12678,27 @@
         <v>0.04</v>
       </c>
       <c r="K18" s="48">
-        <v>3255</v>
+        <v>5000</v>
       </c>
       <c r="M18" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O18" s="24">
         <v>1</v>
       </c>
-      <c r="X18" s="24">
+      <c r="W18" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="19" spans="2:25">
       <c r="B19" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="24">
-        <v>3850</v>
+        <v>3255</v>
       </c>
       <c r="D19" s="24">
-        <v>3850.1</v>
+        <v>3255.1</v>
       </c>
       <c r="E19" s="49">
         <v>1000</v>
@@ -12713,27 +12716,27 @@
         <v>0.04</v>
       </c>
       <c r="K19" s="48">
-        <v>3850</v>
+        <v>3255</v>
       </c>
       <c r="M19" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="W19" s="24">
+        <v>38</v>
+      </c>
+      <c r="O19" s="24">
         <v>1</v>
       </c>
-      <c r="Y19" s="24">
+      <c r="X19" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="20" spans="2:25">
       <c r="B20" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="24">
-        <v>950</v>
+        <v>3850</v>
       </c>
       <c r="D20" s="24">
-        <v>950.1</v>
+        <v>3850.1</v>
       </c>
       <c r="E20" s="49">
         <v>1000</v>
@@ -12751,27 +12754,27 @@
         <v>0.04</v>
       </c>
       <c r="K20" s="48">
-        <v>950</v>
+        <v>3850</v>
       </c>
       <c r="M20" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="U20" s="24">
+        <v>39</v>
+      </c>
+      <c r="W20" s="24">
         <v>1</v>
       </c>
-      <c r="X20" s="24">
+      <c r="Y20" s="24">
         <v>-1</v>
       </c>
     </row>
     <row r="21" spans="2:25">
       <c r="B21" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="24">
-        <v>4850</v>
+        <v>950</v>
       </c>
       <c r="D21" s="24">
-        <v>4850.1000000000004</v>
+        <v>950.1</v>
       </c>
       <c r="E21" s="49">
         <v>1000</v>
@@ -12789,15 +12792,53 @@
         <v>0.04</v>
       </c>
       <c r="K21" s="48">
+        <v>950</v>
+      </c>
+      <c r="M21" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="U21" s="24">
+        <v>1</v>
+      </c>
+      <c r="X21" s="24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25">
+      <c r="B22" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="24">
         <v>4850</v>
       </c>
-      <c r="M21" s="24" t="s">
+      <c r="D22" s="24">
+        <v>4850.1000000000004</v>
+      </c>
+      <c r="E22" s="49">
+        <v>1000</v>
+      </c>
+      <c r="F22" s="24">
+        <v>6000</v>
+      </c>
+      <c r="G22" s="24">
+        <v>0</v>
+      </c>
+      <c r="I22" s="24">
+        <v>35</v>
+      </c>
+      <c r="J22" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="K22" s="48">
+        <v>4850</v>
+      </c>
+      <c r="M22" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="V21" s="24">
+      <c r="V22" s="24">
         <v>1</v>
       </c>
-      <c r="X21" s="24">
+      <c r="X22" s="24">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added documentation to model.gms and static_input.xlsx
</commit_message>
<xml_diff>
--- a/dieterpy/templates/data_input/static_input.xlsx
+++ b/dieterpy/templates/data_input/static_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TUB\02_Git\dieterpy\dieterpy\templates\data_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F5E195-7129-4091-8859-B64C76FE047F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8C014A-14AF-4851-A54D-C9D9C8F26FF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="741" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="741" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LICENSE" sheetId="1" r:id="rId1"/>
@@ -1075,7 +1075,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3216" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3226" uniqueCount="606">
   <si>
     <t>This work is licensed under the Creative Commons Attribution-ShareAlike 4.0 International Public License.</t>
   </si>
@@ -2884,6 +2884,15 @@
   </si>
   <si>
     <t>B4</t>
+  </si>
+  <si>
+    <t>Minimum reservoir outflow relative to installed capacity</t>
+  </si>
+  <si>
+    <t>Maximum reservoir outflow relative to installed capacity</t>
+  </si>
+  <si>
+    <t>Min full-load hours</t>
   </si>
 </sst>
 </file>
@@ -3655,9 +3664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AMJ125"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
@@ -10635,7 +10642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -11579,7 +11586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A2:AMJ34"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -12855,7 +12862,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K5" sqref="K5"/>
+      <selection pane="topRight" activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -21671,10 +21678,10 @@
   <dimension ref="A1:AMJ41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="K6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -23763,8 +23770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22:N23"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -23824,6 +23831,15 @@
       <c r="O1" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="S1" s="1" t="s">
         <v>46</v>
       </c>
@@ -23877,6 +23893,15 @@
       <c r="O2" s="1" t="s">
         <v>149</v>
       </c>
+      <c r="P2" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>605</v>
+      </c>
       <c r="S2" s="1" t="s">
         <v>127</v>
       </c>
@@ -23942,9 +23967,15 @@
       <c r="O4" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+      <c r="P4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="S4" s="24" t="s">
         <v>75</v>
       </c>
@@ -24833,7 +24864,7 @@
   <dimension ref="A1:AMJ109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M91" sqref="M91"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -28567,9 +28598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMJ89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="14.4"/>
   <cols>
@@ -31684,9 +31713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AMJ77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
@@ -32379,8 +32406,8 @@
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -32430,6 +32457,9 @@
       <c r="L1" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="66.75" customHeight="1">
       <c r="A2" s="1" t="s">

</xml_diff>